<commit_message>
added iteration through companies and decryption
</commit_message>
<xml_diff>
--- a/extracted_data/output_Adidas.xlsx
+++ b/extracted_data/output_Adidas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Digitalisierung</t>
   </si>
@@ -32,6 +32,39 @@
   </si>
   <si>
     <t>Internet</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
   </si>
 </sst>
 </file>
@@ -416,8 +449,8 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>2010</v>
+      <c r="A2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -439,8 +472,8 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>2011</v>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -462,8 +495,8 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>2012</v>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -485,8 +518,8 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>2013</v>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -508,8 +541,8 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1">
-        <v>2014</v>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -531,8 +564,8 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="1">
-        <v>2015</v>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -554,8 +587,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1">
-        <v>2016</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -577,8 +610,8 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <v>2017</v>
+      <c r="A9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -600,8 +633,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1">
-        <v>2018</v>
+      <c r="A10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -623,8 +656,8 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>2019</v>
+      <c r="A11" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -646,8 +679,8 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="1">
-        <v>2020</v>
+      <c r="A12" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B12">
         <v>9</v>

</xml_diff>